<commit_message>
updates in results archiving
</commit_message>
<xml_diff>
--- a/Results/Results archive.csv.xlsx
+++ b/Results/Results archive.csv.xlsx
@@ -1,19 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreastheodoulou/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="5800" yWindow="560" windowWidth="36960" windowHeight="16440" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="DataComparison" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DataSets" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="ModelComparison" sheetId="3" r:id="rId6"/>
+    <sheet name="DataComparison" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSets" sheetId="2" r:id="rId2"/>
+    <sheet name="ModelComparison" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>v1</t>
   </si>
@@ -81,13 +97,7 @@
     <t>Catbbost</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Note: </t>
-    </r>
-    <r>
-      <rPr/>
-      <t>For full dataset Gradient Boosting Regressor takes more than 1 hour</t>
-    </r>
+    <t>Note: For full dataset Gradient Boosting Regressor takes more than 1 hour</t>
   </si>
   <si>
     <t>v2</t>
@@ -136,126 +146,97 @@
   </si>
   <si>
     <t>Date_Block_Num = 34</t>
+  </si>
+  <si>
+    <t>TS &amp; Stats Features v2 (from date_block_num &gt;= 17) - for more too large to process</t>
+  </si>
+  <si>
+    <t>3/10</t>
+  </si>
+  <si>
+    <t>5/10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF212121"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF212121"/>
-      <name val="Monospace"/>
-    </font>
-    <font/>
-    <font>
       <b/>
-      <sz val="20.0"/>
+      <sz val="20"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -445,25 +426,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -471,7 +457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -479,7 +465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -496,37 +482,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4">
-        <v>0.373766658391969</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.232825442555617</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.952316008141918</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.948250135515355</v>
-      </c>
-      <c r="E5" s="7">
-        <v>43900.0</v>
-      </c>
-    </row>
-    <row r="7">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>0.37376665839196899</v>
+      </c>
+      <c r="B5">
+        <v>0.23282544255561699</v>
+      </c>
+      <c r="C5">
+        <v>0.95231600814191797</v>
+      </c>
+      <c r="D5">
+        <v>0.94825013551535497</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -534,11 +520,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -551,98 +537,149 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6">
-        <v>0.440703602599847</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0.265142853179263</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.937279531207964</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.928062615894701</v>
-      </c>
-      <c r="E11" s="7">
-        <v>43961.0</v>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>0.44070360259984698</v>
+      </c>
+      <c r="B11">
+        <v>0.26514285317926301</v>
+      </c>
+      <c r="C11">
+        <v>0.93727953120796403</v>
+      </c>
+      <c r="D11">
+        <v>0.92806261589470096</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>0.42</v>
+      </c>
+      <c r="B16">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="C16">
+        <v>0.91920000000000002</v>
+      </c>
+      <c r="D16">
+        <v>0.92200000000000004</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.71"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -650,7 +687,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -659,31 +696,32 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -697,7 +735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -708,10 +746,10 @@
         <v>0.15</v>
       </c>
       <c r="D4" s="3">
-        <v>89.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -722,10 +760,10 @@
         <v>0.12</v>
       </c>
       <c r="D5" s="3">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -736,10 +774,10 @@
         <v>0.1</v>
       </c>
       <c r="D6" s="3">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -747,23 +785,23 @@
         <v>0.25</v>
       </c>
       <c r="C7" s="3">
-        <v>0.149</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="D7" s="3">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates in Time Series Features & modelling code
</commit_message>
<xml_diff>
--- a/Results/Results archive.csv.xlsx
+++ b/Results/Results archive.csv.xlsx
@@ -11,126 +11,162 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgqHXjukAXtt2xNQ2TVBlzXW0eZwg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjFX1OgHOx8qMgFIQNTrMQVkYRWNQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>v1</t>
   </si>
   <si>
+    <t>Small v1 Data set</t>
+  </si>
+  <si>
     <t>DataSets name</t>
   </si>
   <si>
-    <t>Small v1 Data set</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
+    <t>Note: model parameters are default</t>
+  </si>
+  <si>
     <t>TS &amp; Stats Features v1</t>
   </si>
   <si>
+    <t xml:space="preserve">Model </t>
+  </si>
+  <si>
+    <t>XGB</t>
+  </si>
+  <si>
+    <t>Coursera scores</t>
+  </si>
+  <si>
+    <t>Gradient Boosted Decision Trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 train </t>
+  </si>
+  <si>
+    <t>R2 Val</t>
+  </si>
+  <si>
+    <t>RMSE train</t>
+  </si>
+  <si>
+    <t>RMSE val</t>
+  </si>
+  <si>
+    <t>RMSE Test Public</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>RMSE Test Private</t>
+  </si>
+  <si>
+    <t>R2 Train</t>
+  </si>
+  <si>
+    <t>Coursera score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 Val </t>
+  </si>
+  <si>
+    <t>runnig time (seconds)</t>
+  </si>
+  <si>
+    <t>Gradient Boosting Regressor</t>
+  </si>
+  <si>
+    <t>HistGradient Boosting Regressor</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
+  </si>
+  <si>
+    <t>3/10</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>Catbbost</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>Note: For full dataset Gradient Boosting Regressor takes more than 1 hour</t>
+  </si>
+  <si>
+    <t>TS &amp; Stats Features v2 (from date_block_num &gt;= 20) - for more too large to process</t>
+  </si>
+  <si>
+    <t>5/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS &amp; Stats Features v2 </t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
     <t>TS &amp; Stats Features</t>
   </si>
   <si>
-    <t xml:space="preserve">Model </t>
-  </si>
-  <si>
-    <t>XGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 train </t>
-  </si>
-  <si>
-    <t>R2 Val</t>
-  </si>
-  <si>
-    <t>RMSE train</t>
-  </si>
-  <si>
-    <t>RMSE val</t>
-  </si>
-  <si>
-    <t>Note: model parameters are default</t>
-  </si>
-  <si>
-    <t>Coursera score</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>R2 Train</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 Val </t>
-  </si>
-  <si>
-    <t>runnig time (seconds)</t>
-  </si>
-  <si>
-    <t>TS based features: monthly mean of: item price per shop, item price item, item count per shop, item count per item (v1) + item price per item category, item count per item category (v2). For TS features this mean for these features are calculated at different monthly lags (Lags = 1, 3, 6, 12)</t>
-  </si>
-  <si>
-    <t>Gradient Boosting Regressor</t>
+    <t>TS based features: taking monthly mean of item price and item count with respect to follow categories/"groupbys" (i.e grouped by date block num  any other category mentioned) at different lags: 1) items, 2) shops (v1), 3) item category, 4) items &amp; shops, 5) date block num. For TS features this mean for these features are calculated at different monthly lags (Lags = 1, 3, 6, 12). A few exampless of these features include, a  monthly mean of: item price per shop, item price item, item count per shop, item count per item (v1) + item price per item category, item count per item category (v2), item price &amp; count per item and shop, item price &amp; count per date_block_num (v3). For TS features this mean for these features are calculated at different monthly lags (Lags = 1, 3, 6, 12)</t>
   </si>
   <si>
     <t>Stats based features: standard deviation &amp; median of the features defined in TS based features. Only difference is that this stats are only calculated for Lag = 1</t>
   </si>
   <si>
-    <t>HistGradient Boosting Regressor</t>
-  </si>
-  <si>
-    <t>3/10</t>
-  </si>
-  <si>
-    <t>LightGBM</t>
-  </si>
-  <si>
     <t>1)  mean of the 4 following features at different lags (lags = months): item price per shop, item price per item, item count per shop, item count per item. Lags: 1, 2, 3, 6, 12. 2) trends of 1,3,6,12m of the  previous 4 features (item price per shop, item price per item, item cnt per shop, item price per time). 3) binary feature: whether these 4 features are above their average 12m average in the current month (current = lag 1)</t>
   </si>
   <si>
     <t>TS &amp; Stats Features v2</t>
   </si>
   <si>
-    <t>XGBoost</t>
-  </si>
-  <si>
     <t>all of TS &amp; Stats Features v1 + 1) item categories introduced (features per item categories include item price per item categori, and item count per item category). all the features calculated in v1 per shop e.g. are calculated per item category respectively. + 2) the following stats calculated for lag 1 for the 4 features mentioned in v1: standard deviation, median</t>
   </si>
   <si>
-    <t>v2</t>
+    <t>TS &amp; Stats Features v3</t>
+  </si>
+  <si>
+    <t>Same rest of TS &amp; Stats based features only difference features are now also calculated by grouping with 1) items, shops, and date block num, and 2) date block num. Trends have only been calculated for 1m since rest did not have large feature importance</t>
+  </si>
+  <si>
+    <t>TS &amp; Stats Features v4</t>
+  </si>
+  <si>
+    <t>cleaned version of v3</t>
+  </si>
+  <si>
+    <t>TS &amp; Stas features v5</t>
+  </si>
+  <si>
+    <t>Includes the customly made item categories ( 1)manual sorting based on item categories name, 2) NLP and graph-based clustering), and shop categories (manually sorting type of shop based on name given) made by Mike</t>
   </si>
   <si>
     <t>Training dataset</t>
   </si>
   <si>
-    <t>Catbbost</t>
-  </si>
-  <si>
     <t>14&lt;= Date_Block_Num&lt;= 28</t>
   </si>
   <si>
-    <t>Note: For full dataset Gradient Boosting Regressor takes more than 1 hour</t>
-  </si>
-  <si>
     <t>Validation Dataset</t>
   </si>
   <si>
-    <t>TS &amp; Stats Features v2 (from date_block_num &gt;= 20) - for more too large to process</t>
-  </si>
-  <si>
     <t>28&lt;Date_Block_Num &lt;=33</t>
   </si>
   <si>
@@ -140,20 +176,17 @@
     <t>Date_Block_Num = 34</t>
   </si>
   <si>
-    <t>5/10</t>
-  </si>
-  <si>
-    <t>TS &amp; Stats Features v2 (from date_block_num &gt;= 17) - for more too large to process</t>
-  </si>
-  <si>
-    <t>TS &amp; Stats Features v2 (from date_block_num &gt;= 14)</t>
+    <t>TS &amp; Stats v3</t>
+  </si>
+  <si>
+    <t>8/10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -162,12 +195,6 @@
     <font>
       <b/>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -181,13 +208,35 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
       <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
     <font>
+      <b/>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF212121"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -211,22 +260,36 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -466,210 +529,282 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>0.373766658391969</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>0.232825442555617</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="6">
         <v>0.952316008141918</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>0.948250135515355</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>36</v>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="6">
+        <v>0.440703602599847</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.265142853179263</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.937279531207964</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.928062615894701</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="E12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="4">
-        <v>0.440703602599847</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.265142853179263</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.937279531207964</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.928062615894701</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
+      <c r="G15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="3">
+        <v>0.415</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.277</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.9203</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.9204</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="4">
-        <v>0.42</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.274</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.9192</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.922</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="7">
-        <v>0.415</v>
-      </c>
-      <c r="B21" s="7">
-        <v>0.277</v>
-      </c>
-      <c r="C21" s="8">
-        <v>0.9203</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0.9204</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1"/>
+      <c r="H21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.985</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.979</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="H28" s="7"/>
+    </row>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>
     <row r="31" ht="15.75" customHeight="1"/>
@@ -1666,82 +1801,109 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
+      <c r="A1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3"/>
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -2727,6 +2889,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2751,97 +2915,109 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B6" s="2">
         <v>0.24</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C6" s="2">
         <v>0.15</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D6" s="2">
         <v>89.0</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B8" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="2">
         <v>9.0</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.46</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="B9" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.149</v>
+      </c>
+      <c r="D9" s="2">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.149</v>
-      </c>
-      <c r="D7" s="3">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
+    </row>
     <row r="13" ht="15.75" customHeight="1"/>
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>
@@ -3830,6 +4006,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>